<commit_message>
Atualização do banco de dados
</commit_message>
<xml_diff>
--- a/database/Dicionário de Dados.xlsx
+++ b/database/Dicionário de Dados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcmma\Documents\GitHub\BD_Faculdade\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcmma\Documents\GitHub\projeto-faculdade\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823FAAD5-0E28-4AC3-86EF-D778ACA72244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA1A679-1D42-43F9-873E-299C8AD633F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{7322636D-572D-48CD-9664-CDD954481AED}"/>
+    <workbookView xWindow="18504" yWindow="1392" windowWidth="17280" windowHeight="9072" activeTab="1" xr2:uid="{7322636D-572D-48CD-9664-CDD954481AED}"/>
   </bookViews>
   <sheets>
     <sheet name="Entidades" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="190">
   <si>
     <t>DICIONÁRIO DE DADOS: ENTIDADES</t>
   </si>
@@ -465,9 +465,6 @@
     <t>Data de início da disciplina do aluno</t>
   </si>
   <si>
-    <t>8bytes</t>
-  </si>
-  <si>
     <t>Data_Fim</t>
   </si>
   <si>
@@ -495,18 +492,6 @@
     <t>Número de contato do WhatsApp do aluno</t>
   </si>
   <si>
-    <t>Número do telefone celular do aluno</t>
-  </si>
-  <si>
-    <t>Número de contato para recados ao aluno</t>
-  </si>
-  <si>
-    <t>Tel_celular</t>
-  </si>
-  <si>
-    <t>Tel_recado</t>
-  </si>
-  <si>
     <t>Verificar se os campos possuem valores atômicos (somente pode haver um valor em cada campo)</t>
   </si>
   <si>
@@ -517,6 +502,108 @@
   </si>
   <si>
     <t>Verificar se todos os atributos não-chave são dependentes da chave primária. (Não pode haver dependências parciais)</t>
+  </si>
+  <si>
+    <t>Telefones_Aluno</t>
+  </si>
+  <si>
+    <t>Endereço_Aluno</t>
+  </si>
+  <si>
+    <t>Tipo_Logradouro</t>
+  </si>
+  <si>
+    <t>É do tipo</t>
+  </si>
+  <si>
+    <t>Tabela para registro dos endereços dos alunos</t>
+  </si>
+  <si>
+    <t>Tabela de registro dos tipos de logradouros</t>
+  </si>
+  <si>
+    <t>Tipo_Telefone</t>
+  </si>
+  <si>
+    <t>Tabela para registro dos telefones dos alunos</t>
+  </si>
+  <si>
+    <t>Define</t>
+  </si>
+  <si>
+    <t>Descrição dos tipos de telefones aceitos</t>
+  </si>
+  <si>
+    <t>5 bytes</t>
+  </si>
+  <si>
+    <t>11 bytes</t>
+  </si>
+  <si>
+    <t>NOT NULL, UNIQUE</t>
+  </si>
+  <si>
+    <t>Entidade ENDERECO_ALUNO</t>
+  </si>
+  <si>
+    <t>Cod_Endereco</t>
+  </si>
+  <si>
+    <t>Código de idenficação do endereço do aluno</t>
+  </si>
+  <si>
+    <t>Cod_Tipo_Logradouro</t>
+  </si>
+  <si>
+    <t>Código de identificação do tipo de logradouro</t>
+  </si>
+  <si>
+    <t>Complemento</t>
+  </si>
+  <si>
+    <t>20 bytes</t>
+  </si>
+  <si>
+    <t>Complmento(caso houver)</t>
+  </si>
+  <si>
+    <t>Entidade TIPO_LOGRADOURO</t>
+  </si>
+  <si>
+    <t>Nome do tipo de logradouro</t>
+  </si>
+  <si>
+    <t>Cod_Telefone_Aluno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restrições </t>
+  </si>
+  <si>
+    <t>Código de identificação do telefone do aluno</t>
+  </si>
+  <si>
+    <t>Cod_Tipo_Telefone</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>Número do telefone</t>
+  </si>
+  <si>
+    <t>Entidade TIPO_TELEFONE</t>
+  </si>
+  <si>
+    <t>Entidade TELEFONES_ALUNO</t>
+  </si>
+  <si>
+    <t>Código de identificação do tipo de telefone</t>
+  </si>
+  <si>
+    <t>Código de idenficação do aluno</t>
+  </si>
+  <si>
+    <t>Nome do tipo de telefone</t>
   </si>
 </sst>
 </file>
@@ -573,7 +660,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -818,17 +905,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -841,22 +1009,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -865,47 +1023,91 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -916,50 +1118,51 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1275,431 +1478,531 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081B57C7-B96F-4A13-ACB2-E69A8753CDC5}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" style="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="31.88671875" style="57" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1"/>
     <col min="6" max="6" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="58" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="15"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="59"/>
     </row>
     <row r="6" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="30"/>
     </row>
     <row r="8" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="25"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="27"/>
+      <c r="D8" s="31"/>
     </row>
     <row r="9" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="29" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25"/>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="27"/>
+      <c r="D10" s="31"/>
     </row>
     <row r="11" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="29" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="25"/>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="28"/>
+      <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="27"/>
+      <c r="D12" s="31"/>
     </row>
     <row r="13" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="29" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="33"/>
+      <c r="B14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="28"/>
+      <c r="D14" s="30"/>
     </row>
     <row r="15" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="33"/>
+      <c r="B15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="30"/>
     </row>
     <row r="16" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="32"/>
-      <c r="B16" s="18" t="s">
+      <c r="A16" s="51"/>
+      <c r="B16" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="27"/>
+      <c r="D16" s="50"/>
     </row>
     <row r="17" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="29" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="29"/>
-      <c r="B18" s="17" t="s">
+      <c r="A18" s="27"/>
+      <c r="B18" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="28"/>
+      <c r="D18" s="30"/>
     </row>
     <row r="19" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="29"/>
-      <c r="B19" s="17" t="s">
+      <c r="A19" s="27"/>
+      <c r="B19" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="28"/>
-    </row>
-    <row r="20" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
-      <c r="B20" s="18" t="s">
+      <c r="D19" s="30"/>
+    </row>
+    <row r="20" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27"/>
+      <c r="B20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="27"/>
+      <c r="D20" s="30"/>
     </row>
     <row r="21" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="27"/>
+      <c r="B21" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="30"/>
+    </row>
+    <row r="22" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="28"/>
+      <c r="B22" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="31"/>
+    </row>
+    <row r="23" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B23" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C23" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D23" s="54" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="29"/>
-      <c r="B22" s="17" t="s">
+    <row r="24" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="27"/>
+      <c r="B24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C24" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="28"/>
-    </row>
-    <row r="23" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="29"/>
-      <c r="B23" s="17" t="s">
+      <c r="D24" s="30"/>
+    </row>
+    <row r="25" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27"/>
+      <c r="B25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="28"/>
-    </row>
-    <row r="24" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="29"/>
-      <c r="B24" s="17" t="s">
+      <c r="D25" s="30"/>
+    </row>
+    <row r="26" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27"/>
+      <c r="B26" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C26" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="28"/>
-    </row>
-    <row r="25" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="29"/>
-      <c r="B25" s="17" t="s">
+      <c r="D26" s="30"/>
+    </row>
+    <row r="27" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27"/>
+      <c r="B27" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C27" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="28"/>
-    </row>
-    <row r="26" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="25"/>
-      <c r="B26" s="18" t="s">
+      <c r="D27" s="30"/>
+    </row>
+    <row r="28" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="28"/>
+      <c r="B28" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C28" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="27"/>
-    </row>
-    <row r="27" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
+      <c r="D28" s="31"/>
+    </row>
+    <row r="29" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B29" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D29" s="29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="25"/>
-      <c r="B28" s="18" t="s">
+    <row r="30" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="28"/>
+      <c r="B30" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C30" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="27"/>
-    </row>
-    <row r="29" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="24" t="s">
+      <c r="D30" s="31"/>
+    </row>
+    <row r="31" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B31" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C31" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D31" s="29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="25"/>
-      <c r="B30" s="18" t="s">
+    <row r="32" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="28"/>
+      <c r="B32" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C32" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="27"/>
-    </row>
-    <row r="31" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
+      <c r="D32" s="31"/>
+    </row>
+    <row r="33" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B33" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C33" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="D33" s="29" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="25"/>
-      <c r="B32" s="18" t="s">
+    <row r="34" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="28"/>
+      <c r="B34" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C34" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="27"/>
-    </row>
-    <row r="33" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24" t="s">
+      <c r="D34" s="31"/>
+    </row>
+    <row r="35" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B35" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C35" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D35" s="29" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="25"/>
-      <c r="B34" s="18" t="s">
+    <row r="36" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="28"/>
+      <c r="B36" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C36" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="27"/>
-    </row>
-    <row r="35" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="24" t="s">
+      <c r="D36" s="31"/>
+    </row>
+    <row r="37" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B37" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C37" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="26" t="s">
+      <c r="D37" s="29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="25"/>
-      <c r="B36" s="18" t="s">
+    <row r="38" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="48"/>
+      <c r="B38" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C38" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="27"/>
+      <c r="D38" s="50"/>
+    </row>
+    <row r="39" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="28"/>
+      <c r="B40" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D40" s="31"/>
+    </row>
+    <row r="41" spans="1:4" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="B41" s="61" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="62" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="28"/>
+      <c r="B43" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="31"/>
+    </row>
+    <row r="44" spans="1:4" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="B44" s="61" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" s="62" t="s">
+        <v>165</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="27">
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="D23:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="D17:D22"/>
+    <mergeCell ref="A17:A22"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="D21:D26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="A31:A32"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1708,10 +2011,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0621C709-D833-4B1E-A869-0A41CA3D9B62}">
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1720,7 +2023,7 @@
     <col min="2" max="2" width="12.21875" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="58.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.5546875" customWidth="1"/>
     <col min="8" max="8" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -1729,14 +2032,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="47"/>
     </row>
     <row r="3" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -1744,1363 +2047,1698 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
       <c r="H4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I4" s="49" t="s">
-        <v>158</v>
+      <c r="I4" s="22" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="52" t="s">
-        <v>157</v>
+      <c r="I5" s="35" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="52"/>
+      <c r="I6" s="35"/>
     </row>
     <row r="7" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="37"/>
+      <c r="C7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="52"/>
+      <c r="I7" s="35"/>
     </row>
     <row r="8" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43"/>
-      <c r="H9" s="44" t="s">
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
+      <c r="H9" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="I9" s="49" t="s">
-        <v>159</v>
+      <c r="I9" s="22" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="39"/>
+      <c r="C10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="51" t="s">
-        <v>160</v>
+      <c r="I10" s="34" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="39"/>
+      <c r="C11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="51"/>
+      <c r="I11" s="34"/>
     </row>
     <row r="12" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="39"/>
+      <c r="C12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="51"/>
+      <c r="I12" s="34"/>
     </row>
     <row r="13" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="39"/>
+      <c r="C13" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="I13" s="50"/>
+      <c r="I13" s="23"/>
     </row>
     <row r="14" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="39"/>
+      <c r="C14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="14" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="9" t="s">
+      <c r="B15" s="37"/>
+      <c r="C15" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="I15" s="53"/>
+      <c r="I15" s="24"/>
     </row>
     <row r="16" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I16" s="53"/>
+      <c r="I16" s="24"/>
     </row>
     <row r="17" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="43"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="42"/>
       <c r="H17" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I17" s="53"/>
+      <c r="I17" s="24"/>
     </row>
     <row r="18" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="39"/>
+      <c r="C18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="53"/>
+      <c r="I18" s="24"/>
     </row>
     <row r="19" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="39"/>
+      <c r="C19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="14" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="39"/>
+      <c r="C20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="9" t="s">
+      <c r="B21" s="37"/>
+      <c r="C21" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="16" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="43"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="42"/>
       <c r="H23" s="1" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="39"/>
+      <c r="C24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F24" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="4" t="s">
+      <c r="B25" s="39"/>
+      <c r="C25" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" s="14" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="4" t="s">
+      <c r="B26" s="39"/>
+      <c r="C26" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F26" s="14" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="39"/>
+      <c r="C27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" s="4" t="s">
+      <c r="D27" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="14" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="39"/>
+      <c r="C28" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F28" s="14" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="39"/>
+      <c r="C29" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="21" t="s">
+      <c r="F29" s="14" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="9" t="s">
+      <c r="B30" s="37"/>
+      <c r="C30" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="23" t="s">
+      <c r="F30" s="16" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="43"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="42"/>
       <c r="H32" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="37" t="s">
+    <row r="33" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="4" t="s">
+      <c r="B33" s="39"/>
+      <c r="C33" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="F33" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="37" t="s">
+    <row r="34" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="4" t="s">
+      <c r="B34" s="39"/>
+      <c r="C34" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="21" t="s">
+      <c r="F34" s="14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="37" t="s">
+    <row r="35" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="B35" s="38"/>
-      <c r="C35" s="4" t="s">
+      <c r="B35" s="39"/>
+      <c r="C35" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="F35" s="14" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="37" t="s">
+    <row r="36" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="38"/>
-      <c r="C36" s="4" t="s">
+      <c r="B36" s="39"/>
+      <c r="C36" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="F36" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="37" t="s">
+    <row r="37" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="B37" s="38"/>
-      <c r="C37" s="4" t="s">
+      <c r="B37" s="39"/>
+      <c r="C37" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="D37" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="39"/>
+      <c r="C38" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F37" s="21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="38"/>
-      <c r="C38" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E38" s="4" t="s">
+      <c r="F38" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" s="39"/>
+      <c r="C39" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F38" s="21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="37" t="s">
+      <c r="F39" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="39"/>
+      <c r="C40" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="38"/>
-      <c r="C39" s="4" t="s">
+      <c r="B41" s="18"/>
+      <c r="C41" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D41" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E41" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="21" t="s">
+      <c r="F41" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="37" t="s">
+    <row r="42" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="38"/>
-      <c r="C40" s="4" t="s">
+      <c r="B42" s="18"/>
+      <c r="C42" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D42" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E42" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F42" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="37" t="s">
+    <row r="43" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="4" t="s">
+      <c r="B43" s="39"/>
+      <c r="C43" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D43" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E43" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="21" t="s">
+      <c r="F43" s="14" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="4" t="s">
+    <row r="44" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B44" s="18"/>
+      <c r="C44" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D44" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E44" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E45" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F42" s="21" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="4" t="s">
+      <c r="F45" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="63"/>
+    </row>
+    <row r="47" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="42"/>
+      <c r="H47" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="39"/>
+      <c r="C48" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" s="39"/>
+      <c r="C49" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D49" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E49" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50" s="39"/>
+      <c r="C50" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F43" s="21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="B44" s="38"/>
-      <c r="C44" s="4" t="s">
+      <c r="F50" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="39"/>
+      <c r="C51" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E44" s="4" t="s">
+      <c r="D51" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="39"/>
+      <c r="C52" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="39"/>
+      <c r="C53" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F44" s="21" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F45" s="21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="48" t="s">
-        <v>146</v>
-      </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E46" s="4" t="s">
+      <c r="F53" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="37"/>
+      <c r="C54" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E54" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F46" s="21" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="37" t="s">
-        <v>149</v>
-      </c>
-      <c r="B47" s="38"/>
-      <c r="C47" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E47" s="4" t="s">
+      <c r="F54" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="56" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" s="41"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="42"/>
+      <c r="H56" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="39"/>
+      <c r="C57" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="39"/>
+      <c r="C58" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59" s="39"/>
+      <c r="C59" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" s="44"/>
+      <c r="C60" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F47" s="21" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="37" t="s">
-        <v>150</v>
-      </c>
-      <c r="B48" s="38"/>
-      <c r="C48" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E48" s="4" t="s">
+      <c r="F60" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B61" s="37"/>
+      <c r="C61" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E61" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F48" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="37" t="s">
-        <v>155</v>
-      </c>
-      <c r="B49" s="38"/>
-      <c r="C49" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E49" s="4" t="s">
+      <c r="F61" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="63" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="41"/>
+      <c r="C63" s="41"/>
+      <c r="D63" s="41"/>
+      <c r="E63" s="41"/>
+      <c r="F63" s="42"/>
+      <c r="H63" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B64" s="39"/>
+      <c r="C64" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="B65" s="39"/>
+      <c r="C65" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" s="39"/>
+      <c r="C66" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67" s="39"/>
+      <c r="C67" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F49" s="21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="B50" s="40"/>
-      <c r="C50" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="F50" s="23" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="52" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="B52" s="42"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="43"/>
-      <c r="H52" s="1" t="s">
+      <c r="F67" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" s="37"/>
+      <c r="C68" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="70" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" s="41"/>
+      <c r="C70" s="41"/>
+      <c r="D70" s="41"/>
+      <c r="E70" s="41"/>
+      <c r="F70" s="42"/>
+      <c r="H70" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="37" t="s">
+    <row r="71" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="38"/>
-      <c r="C53" s="4" t="s">
+      <c r="B71" s="39"/>
+      <c r="C71" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D71" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E71" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F53" s="21" t="s">
+      <c r="F71" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="37" t="s">
+    <row r="72" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="39"/>
+      <c r="C72" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F72" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="B54" s="38"/>
-      <c r="C54" s="4" t="s">
+      <c r="B73" s="37"/>
+      <c r="C73" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D73" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F54" s="21" t="s">
+      <c r="E73" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F73" s="16" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="B55" s="38"/>
-      <c r="C55" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F55" s="21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="38"/>
-      <c r="C56" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F56" s="21" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B57" s="38"/>
-      <c r="C57" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F57" s="21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="B58" s="38"/>
-      <c r="C58" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F58" s="21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="B59" s="40"/>
-      <c r="C59" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F59" s="23" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="61" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="B61" s="42"/>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="43"/>
-      <c r="H61" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B62" s="38"/>
-      <c r="C62" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F62" s="21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="B63" s="38"/>
-      <c r="C63" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F63" s="21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="B64" s="38"/>
-      <c r="C64" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F64" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" s="46"/>
-      <c r="C65" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F65" s="47" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="B66" s="40"/>
-      <c r="C66" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F66" s="23" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="68" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="B68" s="42"/>
-      <c r="C68" s="42"/>
-      <c r="D68" s="42"/>
-      <c r="E68" s="42"/>
-      <c r="F68" s="43"/>
-      <c r="H68" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B69" s="38"/>
-      <c r="C69" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F69" s="21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="B70" s="38"/>
-      <c r="C70" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F70" s="21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="B71" s="38"/>
-      <c r="C71" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F71" s="21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="B72" s="38"/>
-      <c r="C72" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F72" s="21" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="B73" s="40"/>
-      <c r="C73" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F73" s="23" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="75" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="B75" s="42"/>
-      <c r="C75" s="42"/>
-      <c r="D75" s="42"/>
-      <c r="E75" s="42"/>
-      <c r="F75" s="43"/>
+      <c r="A75" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B75" s="41"/>
+      <c r="C75" s="41"/>
+      <c r="D75" s="41"/>
+      <c r="E75" s="41"/>
+      <c r="F75" s="42"/>
       <c r="H75" s="1" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="37" t="s">
+      <c r="A76" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="38"/>
-      <c r="C76" s="4" t="s">
+      <c r="B76" s="39"/>
+      <c r="C76" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="D76" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E76" s="4" t="s">
+      <c r="E76" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F76" s="21" t="s">
+      <c r="F76" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B77" s="38"/>
-      <c r="C77" s="4" t="s">
+      <c r="A77" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B77" s="39"/>
+      <c r="C77" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E77" s="4" t="s">
+      <c r="E77" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F77" s="21" t="s">
-        <v>72</v>
+      <c r="F77" s="14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="39" t="s">
+      <c r="A78" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="B78" s="40"/>
-      <c r="C78" s="9" t="s">
+      <c r="B78" s="37"/>
+      <c r="C78" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D78" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E78" s="9" t="s">
+      <c r="E78" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F78" s="23" t="s">
+      <c r="F78" s="16" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="80" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="B80" s="42"/>
-      <c r="C80" s="42"/>
-      <c r="D80" s="42"/>
-      <c r="E80" s="42"/>
-      <c r="F80" s="43"/>
+      <c r="A80" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B80" s="41"/>
+      <c r="C80" s="41"/>
+      <c r="D80" s="41"/>
+      <c r="E80" s="41"/>
+      <c r="F80" s="42"/>
       <c r="H80" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="37" t="s">
+    <row r="81" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B81" s="38"/>
-      <c r="C81" s="4" t="s">
+      <c r="B81" s="39"/>
+      <c r="C81" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D81" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E81" s="4" t="s">
+      <c r="E81" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F81" s="21" t="s">
+      <c r="F81" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B82" s="38"/>
-      <c r="C82" s="4" t="s">
+    <row r="82" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82" s="39"/>
+      <c r="C82" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="D82" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B83" s="37"/>
+      <c r="C83" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D83" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E82" s="4" t="s">
+      <c r="E83" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F82" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="B83" s="40"/>
-      <c r="C83" s="9" t="s">
+      <c r="F83" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="85" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="B85" s="41"/>
+      <c r="C85" s="41"/>
+      <c r="D85" s="41"/>
+      <c r="E85" s="41"/>
+      <c r="F85" s="42"/>
+    </row>
+    <row r="86" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B86" s="39"/>
+      <c r="C86" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F86" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="B87" s="39"/>
+      <c r="C87" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D83" s="9" t="s">
+      <c r="D87" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F87" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B88" s="39"/>
+      <c r="C88" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F88" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="B89" s="39"/>
+      <c r="C89" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F89" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B90" s="18"/>
+      <c r="C90" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F90" s="14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="B91" s="39"/>
+      <c r="C91" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D91" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E83" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F83" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="85" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="B85" s="42"/>
-      <c r="C85" s="42"/>
-      <c r="D85" s="42"/>
-      <c r="E85" s="42"/>
-      <c r="F85" s="43"/>
-      <c r="H85" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="37" t="s">
+      <c r="E91" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F91" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B92" s="18"/>
+      <c r="C92" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B93" s="37"/>
+      <c r="C93" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F93" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="95" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B95" s="41"/>
+      <c r="C95" s="41"/>
+      <c r="D95" s="41"/>
+      <c r="E95" s="41"/>
+      <c r="F95" s="42"/>
+    </row>
+    <row r="96" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B86" s="38"/>
-      <c r="C86" s="4" t="s">
+      <c r="B96" s="39"/>
+      <c r="C96" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="D96" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="E96" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F86" s="21" t="s">
+      <c r="F96" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="37" t="s">
+    <row r="97" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="B97" s="39"/>
+      <c r="C97" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F97" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="B98" s="37"/>
+      <c r="C98" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E98" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F98" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="100" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="B100" s="41"/>
+      <c r="C100" s="41"/>
+      <c r="D100" s="41"/>
+      <c r="E100" s="41"/>
+      <c r="F100" s="42"/>
+    </row>
+    <row r="101" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B101" s="39"/>
+      <c r="C101" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F101" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="B102" s="39"/>
+      <c r="C102" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F102" s="14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="B87" s="38"/>
-      <c r="C87" s="4" t="s">
+      <c r="B103" s="39"/>
+      <c r="C103" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D103" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E87" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F87" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="B88" s="40"/>
-      <c r="C88" s="9" t="s">
+      <c r="E103" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F103" s="14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="B104" s="39"/>
+      <c r="C104" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D88" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F88" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
+      <c r="D104" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F104" s="14" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="B105" s="37"/>
+      <c r="C105" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E105" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F105" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="65"/>
+      <c r="B106" s="65"/>
+    </row>
+    <row r="107" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="B107" s="41"/>
+      <c r="C107" s="41"/>
+      <c r="D107" s="41"/>
+      <c r="E107" s="41"/>
+      <c r="F107" s="42"/>
+    </row>
+    <row r="108" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B108" s="39"/>
+      <c r="C108" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F108" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="B109" s="39"/>
+      <c r="C109" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F109" s="14" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="B110" s="37"/>
+      <c r="C110" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E110" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F110" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" ht="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="75">
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="I5:I7"/>
+  <mergeCells count="90">
+    <mergeCell ref="A107:F107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A95:F95"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A100:F100"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A80:F80"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A51:B51"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A33:B33"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A17:F17"/>
@@ -3114,39 +3752,32 @@
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A80:F80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A85:F85"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A21:B21"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>